<commit_message>
SFC strings to value starts to work
</commit_message>
<xml_diff>
--- a/SFC_Country.xlsx
+++ b/SFC_Country.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DC1140B-37D4-4DF1-942D-2F62878AB10F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC3BD09-608E-49FC-89CF-BAE4BFF7A10C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5484" yWindow="468" windowWidth="15996" windowHeight="11784" xr2:uid="{1CC8407C-9C85-4F80-BB08-BE5BF0A7339A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{1CC8407C-9C85-4F80-BB08-BE5BF0A7339A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
   <si>
     <t>SFC Country Group</t>
   </si>
@@ -246,6 +246,18 @@
   </si>
   <si>
     <t>BBG Country Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China - Hong Kong </t>
+  </si>
+  <si>
+    <t>China - Mainland</t>
+  </si>
+  <si>
+    <t>China - Macau</t>
+  </si>
+  <si>
+    <t>China - Taiwan</t>
   </si>
 </sst>
 </file>
@@ -608,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6ADEE6C-730C-4A53-9570-3F6A1031B05A}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,7 +793,7 @@
         <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -836,7 +848,7 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -869,7 +881,7 @@
         <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -946,7 +958,7 @@
         <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1205,18 +1217,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1239,14 +1251,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F344AA7-7E24-4E49-AFAE-48D08A417130}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C6C3F01-EAF3-493B-BE4C-0AE96D2DD289}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -1261,4 +1265,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F344AA7-7E24-4E49-AFAE-48D08A417130}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>